<commit_message>
Rewrite data in task_5_data.xlsx
</commit_message>
<xml_diff>
--- a/rlezhaiko/lesson_6/task_5_data.xlsx
+++ b/rlezhaiko/lesson_6/task_5_data.xlsx
@@ -462,32 +462,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>492315</t>
+          <t>836942</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>605792</t>
+          <t>727809</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>519655</t>
+          <t>949621</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>824501</t>
+          <t>573574</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>457707</t>
+          <t>733386</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>541978</t>
+          <t>803444</t>
         </is>
       </c>
     </row>
@@ -536,32 +536,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>560-7-74</t>
+          <t>522-0-1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>508-54-34</t>
+          <t>837-85-44</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>772-24-7</t>
+          <t>407-81-47</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>937-23-19</t>
+          <t>324-24-64</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>735-51-6</t>
+          <t>400-96-1</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>116-42-94</t>
+          <t>661-43-96</t>
         </is>
       </c>
     </row>

</xml_diff>